<commit_message>
working poller and processor for jobtitleparser
</commit_message>
<xml_diff>
--- a/py/website_map.xlsx
+++ b/py/website_map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\burtn\Development\py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF5876A-3794-4044-A5BB-BE98AFAFA629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9ED03C-069F-4A56-A161-F873C0C7928C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{A22F8572-4AAC-4537-969F-985CD15C3299}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="250">
   <si>
     <t>_date</t>
   </si>
@@ -1028,6 +1028,24 @@
   </si>
   <si>
     <t>launchstartups_bnp_goes_live_with_cosmos</t>
+  </si>
+  <si>
+    <t>`14 Dec 23</t>
+  </si>
+  <si>
+    <t>`E:\new_onedrive\Velox Financial Technology\Velox Shared Drive - Documents\General\Marketing &amp; Branding\Content\Blogposts\5675175640 - posting FIX event interview\Website_Final.png</t>
+  </si>
+  <si>
+    <t>Buy &amp; Build is the Future : Interview w/Jon Butler</t>
+  </si>
+  <si>
+    <t>buy_build_interview_with_jon</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/feed/update/urn:li:activity:7141024832518811648</t>
+  </si>
+  <si>
+    <t>Live from the FIX Americas Trading Conference, Toby is joined by Jon Butler, Co-Founder and CEO at Velox. Jon highlights the importance of combining buying and building strategies for development platforms to foster innovation in banking technology</t>
   </si>
 </sst>
 </file>
@@ -1620,11 +1638,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CF13ED-462C-4CD3-93B8-B610EC93C7BB}">
-  <dimension ref="A1:AL33"/>
+  <dimension ref="A1:AM33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N1" sqref="N1"/>
+      <pane xSplit="1" topLeftCell="AJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AM5" sqref="AM5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1643,9 +1661,10 @@
     <col min="29" max="30" width="45" customWidth="1"/>
     <col min="31" max="31" width="107.21875" customWidth="1"/>
     <col min="32" max="38" width="45" customWidth="1"/>
+    <col min="39" max="39" width="56.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="15" t="s">
         <v>7</v>
       </c>
@@ -1754,8 +1773,11 @@
       <c r="AL1" s="20" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="2" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AM1" s="20" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1867,8 +1889,11 @@
       <c r="AL2" s="16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AM2" s="18" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>22</v>
       </c>
@@ -1976,8 +2001,11 @@
       <c r="AL3" s="16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:38" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AM3" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
@@ -2089,8 +2117,11 @@
       <c r="AL4" s="8" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="5" spans="1:38" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AM4" s="8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
@@ -2202,8 +2233,11 @@
       <c r="AL5" s="16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AM5" s="8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>14</v>
       </c>
@@ -2315,8 +2349,11 @@
       <c r="AL6" s="8" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="7" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AM6" s="8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
@@ -2428,8 +2465,11 @@
       <c r="AL7" s="25" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="8" spans="1:38" ht="127.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AM7" s="25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" ht="127.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
@@ -2541,8 +2581,11 @@
       <c r="AL8" s="22" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="9" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AM8" s="24" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>44</v>
       </c>
@@ -2654,8 +2697,11 @@
       <c r="AL9" s="22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AM9" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>45</v>
       </c>
@@ -2767,8 +2813,11 @@
       <c r="AL10" s="22" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="11" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AM10" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>4</v>
       </c>
@@ -2880,8 +2929,11 @@
       <c r="AL11" s="8" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="12" spans="1:38" ht="370.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AM11" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" ht="370.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>16</v>
       </c>
@@ -2993,8 +3045,11 @@
       <c r="AL12" s="16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AM12" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>21</v>
       </c>
@@ -3106,10 +3161,13 @@
       <c r="AL13" s="8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="14" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="AM13" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="6:6" x14ac:dyDescent="0.3">
@@ -3121,18 +3179,19 @@
     <hyperlink ref="M8" r:id="rId1" xr:uid="{F4FBC4A4-D421-41A3-BC25-AC0B9DBA525C}"/>
     <hyperlink ref="AA8" r:id="rId2" xr:uid="{1D6563FB-75D2-4BC1-9BEA-EB2AF7F8ADAD}"/>
     <hyperlink ref="Z8" r:id="rId3" xr:uid="{6F333167-CA9F-48BB-8185-40AC8AD9C9AC}"/>
+    <hyperlink ref="AM8" r:id="rId4" xr:uid="{C6AF4D09-1217-463B-9654-EA374F7BCE3A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF8BF56B-BD18-4506-ADAF-6D00AFC72B81}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3541,6 +3600,20 @@
         <v>15</v>
       </c>
     </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3548,10 +3621,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D13F250-6BF2-432B-8BBD-37DD2CB7E187}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3953,6 +4026,14 @@
         <v>80</v>
       </c>
     </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3960,10 +4041,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45696BE3-9D2F-4C38-9762-C431A9CE78FC}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4246,6 +4327,14 @@
         <v>82</v>
       </c>
     </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4253,10 +4342,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B0980F-5ABF-4EE3-A388-69FF239E9C6C}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4323,9 +4412,6 @@
       <c r="A12" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
@@ -4427,29 +4513,37 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -4462,7 +4556,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D13"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>